<commit_message>
added BubblerPrecursor class in MOVPE
</commit_message>
<xml_diff>
--- a/IKZ_plugin/tests/data/movpe/movpe2/GaO.growth.movpe.ikz.xlsx
+++ b/IKZ_plugin/tests/data/movpe/movpe2/GaO.growth.movpe.ikz.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GrowthRun" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GrowthRun" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="88">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t xml:space="preserve">Molar Flux calculated from partial pressure and flows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow Rate of TEGa + Argon from MFC (Mass Flow Controller, MFC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The back-pressure in the tube carrying the bubbler material. Total Pressure Ar + TEGa</t>
   </si>
   <si>
     <t xml:space="preserve">Oxidant material</t>
@@ -294,7 +300,7 @@
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -412,11 +418,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -523,7 +524,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -728,10 +729,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,6 +840,112 @@
 </externalLink>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -850,8 +953,8 @@
   </sheetPr>
   <dimension ref="A1:ALT14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI18" activeCellId="0" sqref="AI18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK10" activeCellId="0" sqref="AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1262,10 +1365,10 @@
         <v>30</v>
       </c>
       <c r="AA7" s="24" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="AB7" s="23" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="AC7" s="23" t="s">
         <v>33</v>
@@ -1284,10 +1387,10 @@
         <v>37</v>
       </c>
       <c r="AI7" s="24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AJ7" s="24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AK7" s="24"/>
       <c r="AL7" s="25"/>
@@ -1297,7 +1400,7 @@
     </row>
     <row r="8" s="5" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
@@ -1311,118 +1414,118 @@
     </row>
     <row r="9" s="41" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M9" s="31" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N9" s="33" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P9" s="34" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R9" s="35" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="S9" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="T9" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="U9" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="W9" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="X9" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z9" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="T9" s="35" t="s">
+      <c r="AA9" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="U9" s="35" t="s">
+      <c r="AB9" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="V9" s="35" t="s">
+      <c r="AC9" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="AD9" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="X9" s="35" t="s">
+      <c r="AE9" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="Y9" s="35" t="s">
+      <c r="AF9" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="Z9" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA9" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB9" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC9" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD9" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE9" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF9" s="36" t="s">
-        <v>63</v>
-      </c>
       <c r="AG9" s="36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AH9" s="36" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AI9" s="37" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AJ9" s="38" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AK9" s="37" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AL9" s="39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AM9" s="14"/>
       <c r="AN9" s="14"/>
@@ -2397,19 +2500,19 @@
     </row>
     <row r="10" s="41" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F10" s="43" t="n">
         <v>8</v>
@@ -2446,7 +2549,7 @@
         <v>80</v>
       </c>
       <c r="Q10" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R10" s="45" t="n">
         <v>30</v>
@@ -2465,11 +2568,11 @@
         <v>6.80402951697616</v>
       </c>
       <c r="Y10" s="48" t="n">
-        <f aca="false">(R10*X10)/((R10-X10)*22400)</f>
-        <v>0.00039285010895895</v>
+        <f aca="false">(R10*X10)/((S10-X10)*22400)</f>
+        <v>9.17496627300328E-006</v>
       </c>
       <c r="Z10" s="49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA10" s="45" t="n">
         <v>900</v>
@@ -2498,7 +2601,7 @@
         <v>2.03822378435889E-009</v>
       </c>
       <c r="AI10" s="49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AJ10" s="11" t="n">
         <v>500</v>
@@ -2508,7 +2611,7 @@
         <v>0.0223214285714286</v>
       </c>
       <c r="AL10" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AM10" s="40"/>
       <c r="AN10" s="40"/>
@@ -3483,19 +3586,19 @@
     </row>
     <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F11" s="43" t="n">
         <v>8</v>
@@ -3503,7 +3606,7 @@
       <c r="G11" s="11" t="n">
         <v>210</v>
       </c>
-      <c r="H11" s="51" t="n">
+      <c r="H11" s="44" t="n">
         <v>840</v>
       </c>
       <c r="I11" s="44" t="n">
@@ -3532,7 +3635,7 @@
         <v>80</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R11" s="45" t="n">
         <v>30</v>
@@ -3551,11 +3654,11 @@
         <v>6.80402951697616</v>
       </c>
       <c r="Y11" s="48" t="n">
-        <f aca="false">(R11*X11)/((R11-X11)*22400)</f>
-        <v>0.00039285010895895</v>
+        <f aca="false">(R11*X11)/((S11-X11)*22400)</f>
+        <v>9.17496627300328E-006</v>
       </c>
       <c r="Z11" s="49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA11" s="45" t="n">
         <v>900</v>
@@ -3584,7 +3687,7 @@
         <v>2.03822378435889E-009</v>
       </c>
       <c r="AI11" s="49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AJ11" s="11" t="n">
         <v>500</v>
@@ -3594,7 +3697,7 @@
         <v>0.0223214285714286</v>
       </c>
       <c r="AL11" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AM11" s="40"/>
       <c r="AN11" s="40"/>
@@ -4569,19 +4672,19 @@
     </row>
     <row r="12" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F12" s="43" t="n">
         <v>8</v>
@@ -4618,7 +4721,7 @@
         <v>70</v>
       </c>
       <c r="Q12" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R12" s="45" t="n">
         <v>32</v>
@@ -4637,11 +4740,11 @@
         <v>32.9183978916656</v>
       </c>
       <c r="Y12" s="48" t="n">
-        <f aca="false">(R12*X12)/((R12-X12)*22400)</f>
-        <v>-0.0512046936618006</v>
+        <f aca="false">(R12*X12)/((S12-X12)*22400)</f>
+        <v>4.0293911426096E-005</v>
       </c>
       <c r="Z12" s="49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA12" s="45" t="n">
         <v>700</v>
@@ -4670,7 +4773,7 @@
         <v>2.36113415510719E-008</v>
       </c>
       <c r="AI12" s="49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AJ12" s="11" t="n">
         <v>700</v>
@@ -4680,7 +4783,7 @@
         <v>0.03125</v>
       </c>
       <c r="AL12" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AM12" s="40"/>
       <c r="AN12" s="40"/>
@@ -5655,19 +5758,19 @@
     </row>
     <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F13" s="43" t="n">
         <v>8</v>
@@ -5704,7 +5807,7 @@
         <v>70</v>
       </c>
       <c r="Q13" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R13" s="45" t="n">
         <v>32</v>
@@ -5723,11 +5826,11 @@
         <v>32.9183978916656</v>
       </c>
       <c r="Y13" s="48" t="n">
-        <f aca="false">(R13*X13)/((R13-X13)*22400)</f>
-        <v>-0.0512046936618006</v>
+        <f aca="false">(R13*X13)/((S13-X13)*22400)</f>
+        <v>4.0293911426096E-005</v>
       </c>
       <c r="Z13" s="49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA13" s="45" t="n">
         <v>700</v>
@@ -5756,7 +5859,7 @@
         <v>2.36113415510719E-008</v>
       </c>
       <c r="AI13" s="49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AJ13" s="11" t="n">
         <v>700</v>
@@ -5766,7 +5869,7 @@
         <v>0.03125</v>
       </c>
       <c r="AL13" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AM13" s="40"/>
       <c r="AN13" s="40"/>
@@ -6741,19 +6844,19 @@
     </row>
     <row r="14" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>82</v>
-      </c>
       <c r="E14" s="43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F14" s="43" t="n">
         <v>9</v>
@@ -6790,7 +6893,7 @@
         <v>70</v>
       </c>
       <c r="Q14" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="R14" s="45" t="n">
         <v>32</v>
@@ -6809,11 +6912,11 @@
         <v>32.9183978916656</v>
       </c>
       <c r="Y14" s="48" t="n">
-        <f aca="false">(R14*X14)/((R14-X14)*22400)</f>
-        <v>-0.0512046936618006</v>
+        <f aca="false">(R14*X14)/((S14-X14)*22400)</f>
+        <v>4.0293911426096E-005</v>
       </c>
       <c r="Z14" s="49" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA14" s="45" t="n">
         <v>700</v>
@@ -6842,7 +6945,7 @@
         <v>2.36113415510719E-008</v>
       </c>
       <c r="AI14" s="49" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AJ14" s="11" t="n">
         <v>700</v>
@@ -6852,7 +6955,7 @@
         <v>0.03125</v>
       </c>
       <c r="AL14" s="50" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AM14" s="40"/>
       <c r="AN14" s="40"/>

</xml_diff>